<commit_message>
starting process to add change from last week
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -6,7 +6,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="results_sheet" r:id="rId3" sheetId="1"/>
+    <sheet name="Week1" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
@@ -29,46 +29,46 @@
     <t/>
   </si>
   <si>
+    <t>DJ's Quality Team</t>
+  </si>
+  <si>
+    <t>Samsquanches</t>
+  </si>
+  <si>
+    <t>Sánteros</t>
+  </si>
+  <si>
+    <t>Lundo’s Legends</t>
+  </si>
+  <si>
+    <t>SmokeWalkers</t>
+  </si>
+  <si>
+    <t>Swampnuts</t>
+  </si>
+  <si>
+    <t>GOD WILLS IT</t>
+  </si>
+  <si>
+    <t>MillerTime</t>
+  </si>
+  <si>
+    <t>PrimeTime</t>
+  </si>
+  <si>
+    <t>confusion</t>
+  </si>
+  <si>
     <t>rainmaker</t>
   </si>
   <si>
-    <t>GOD WILLS IT</t>
-  </si>
-  <si>
-    <t>swampnuts</t>
-  </si>
-  <si>
-    <t>osi's seal clubbers</t>
-  </si>
-  <si>
-    <t>Lundo's Legends</t>
-  </si>
-  <si>
-    <t>fausty is gay</t>
-  </si>
-  <si>
-    <t>Fly Ballin'</t>
-  </si>
-  <si>
-    <t>SCOTT_THE_TANK</t>
-  </si>
-  <si>
     <t>Epic7</t>
   </si>
   <si>
-    <t>HOW'S-YOUR-ASPEN?</t>
-  </si>
-  <si>
-    <t>Weebs</t>
-  </si>
-  <si>
-    <t>Hamilton's Killers</t>
-  </si>
-  <si>
-    <t>Smoke18</t>
-  </si>
-  <si>
-    <t>confusion</t>
+    <t>KING JOSEPH 1 3 1</t>
+  </si>
+  <si>
+    <t>Splitfinger Skadoosh</t>
   </si>
 </sst>
 </file>
@@ -147,13 +147,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>141.0</v>
+        <v>120.0</v>
       </c>
       <c r="C2" t="n">
-        <v>78.0</v>
+        <v>59.0</v>
       </c>
       <c r="D2" t="n">
-        <v>63.0</v>
+        <v>61.0</v>
       </c>
     </row>
     <row r="3">
@@ -161,13 +161,13 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>139.0</v>
+        <v>116.5</v>
       </c>
       <c r="C3" t="n">
-        <v>71.0</v>
+        <v>70.5</v>
       </c>
       <c r="D3" t="n">
-        <v>68.0</v>
+        <v>46.0</v>
       </c>
     </row>
     <row r="4">
@@ -175,13 +175,13 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>132.0</v>
+        <v>112.5</v>
       </c>
       <c r="C4" t="n">
-        <v>74.5</v>
+        <v>70.0</v>
       </c>
       <c r="D4" t="n">
-        <v>57.5</v>
+        <v>42.5</v>
       </c>
     </row>
     <row r="5">
@@ -189,13 +189,13 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>103.5</v>
+        <v>105.5</v>
       </c>
       <c r="C5" t="n">
-        <v>46.0</v>
+        <v>54.5</v>
       </c>
       <c r="D5" t="n">
-        <v>57.5</v>
+        <v>51.0</v>
       </c>
     </row>
     <row r="6">
@@ -203,13 +203,13 @@
         <v>9</v>
       </c>
       <c r="B6" t="n">
-        <v>103.5</v>
+        <v>101.5</v>
       </c>
       <c r="C6" t="n">
-        <v>47.5</v>
+        <v>64.0</v>
       </c>
       <c r="D6" t="n">
-        <v>56.0</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="7">
@@ -217,13 +217,13 @@
         <v>10</v>
       </c>
       <c r="B7" t="n">
-        <v>90.0</v>
+        <v>98.0</v>
       </c>
       <c r="C7" t="n">
-        <v>46.0</v>
+        <v>38.5</v>
       </c>
       <c r="D7" t="n">
-        <v>44.0</v>
+        <v>59.5</v>
       </c>
     </row>
     <row r="8">
@@ -231,13 +231,13 @@
         <v>11</v>
       </c>
       <c r="B8" t="n">
-        <v>86.0</v>
+        <v>88.0</v>
       </c>
       <c r="C8" t="n">
-        <v>30.5</v>
+        <v>44.0</v>
       </c>
       <c r="D8" t="n">
-        <v>55.5</v>
+        <v>44.0</v>
       </c>
     </row>
     <row r="9">
@@ -245,13 +245,13 @@
         <v>12</v>
       </c>
       <c r="B9" t="n">
-        <v>84.5</v>
+        <v>85.0</v>
       </c>
       <c r="C9" t="n">
-        <v>49.5</v>
+        <v>37.0</v>
       </c>
       <c r="D9" t="n">
-        <v>35.0</v>
+        <v>48.0</v>
       </c>
     </row>
     <row r="10">
@@ -259,13 +259,13 @@
         <v>13</v>
       </c>
       <c r="B10" t="n">
-        <v>79.0</v>
+        <v>83.0</v>
       </c>
       <c r="C10" t="n">
         <v>51.5</v>
       </c>
       <c r="D10" t="n">
-        <v>27.5</v>
+        <v>31.5</v>
       </c>
     </row>
     <row r="11">
@@ -273,13 +273,13 @@
         <v>14</v>
       </c>
       <c r="B11" t="n">
-        <v>71.5</v>
+        <v>81.0</v>
       </c>
       <c r="C11" t="n">
-        <v>20.0</v>
+        <v>47.0</v>
       </c>
       <c r="D11" t="n">
-        <v>51.5</v>
+        <v>34.0</v>
       </c>
     </row>
     <row r="12">
@@ -287,13 +287,13 @@
         <v>15</v>
       </c>
       <c r="B12" t="n">
-        <v>61.5</v>
+        <v>72.0</v>
       </c>
       <c r="C12" t="n">
-        <v>26.5</v>
+        <v>28.5</v>
       </c>
       <c r="D12" t="n">
-        <v>35.0</v>
+        <v>43.5</v>
       </c>
     </row>
     <row r="13">
@@ -301,13 +301,13 @@
         <v>16</v>
       </c>
       <c r="B13" t="n">
-        <v>60.0</v>
+        <v>70.5</v>
       </c>
       <c r="C13" t="n">
-        <v>35.0</v>
+        <v>32.0</v>
       </c>
       <c r="D13" t="n">
-        <v>25.0</v>
+        <v>38.5</v>
       </c>
     </row>
     <row r="14">
@@ -315,13 +315,13 @@
         <v>17</v>
       </c>
       <c r="B14" t="n">
-        <v>56.5</v>
+        <v>67.5</v>
       </c>
       <c r="C14" t="n">
-        <v>38.5</v>
+        <v>16.0</v>
       </c>
       <c r="D14" t="n">
-        <v>18.0</v>
+        <v>51.5</v>
       </c>
     </row>
     <row r="15">
@@ -329,13 +329,13 @@
         <v>18</v>
       </c>
       <c r="B15" t="n">
-        <v>52.0</v>
+        <v>59.0</v>
       </c>
       <c r="C15" t="n">
-        <v>15.5</v>
+        <v>17.5</v>
       </c>
       <c r="D15" t="n">
-        <v>36.5</v>
+        <v>41.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Brewster] small, unimportant changes
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -6,7 +6,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Week1" r:id="rId3" sheetId="1"/>
+    <sheet name="Week15" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
@@ -41,46 +41,46 @@
     <t/>
   </si>
   <si>
-    <t>overRated vs Audigy Scum</t>
-  </si>
-  <si>
     <t>Lundo’s Legends</t>
   </si>
   <si>
+    <t>EL Onće</t>
+  </si>
+  <si>
+    <t>Epic7</t>
+  </si>
+  <si>
+    <t>Samsquanches</t>
+  </si>
+  <si>
+    <t>Splitfinger Skadoosh</t>
+  </si>
+  <si>
+    <t>confusion</t>
+  </si>
+  <si>
+    <t>SmokeWalkers</t>
+  </si>
+  <si>
+    <t>GOD WILLS IT</t>
+  </si>
+  <si>
+    <t>DJ's Quality Team</t>
+  </si>
+  <si>
+    <t>rainmaker</t>
+  </si>
+  <si>
+    <t>Swampnuts</t>
+  </si>
+  <si>
+    <t>MillerTime</t>
+  </si>
+  <si>
+    <t>Corbin Copy</t>
+  </si>
+  <si>
     <t>Mac</t>
-  </si>
-  <si>
-    <t>rainmaker</t>
-  </si>
-  <si>
-    <t>Splitfinger Skadoosh</t>
-  </si>
-  <si>
-    <t>GOD WILLS IT</t>
-  </si>
-  <si>
-    <t>Swampnuts</t>
-  </si>
-  <si>
-    <t>Corbin Copy</t>
-  </si>
-  <si>
-    <t>EL Onće</t>
-  </si>
-  <si>
-    <t>DJ's Quality Team</t>
-  </si>
-  <si>
-    <t>SmokeWalkers</t>
-  </si>
-  <si>
-    <t>confusion</t>
-  </si>
-  <si>
-    <t>Samsquanches</t>
-  </si>
-  <si>
-    <t>MillerTime</t>
   </si>
 </sst>
 </file>
@@ -174,22 +174,22 @@
         <v>9</v>
       </c>
       <c r="C2" t="n">
-        <v>125.0</v>
+        <v>131.0</v>
       </c>
       <c r="D2" t="n">
-        <v>68.5</v>
+        <v>57.0</v>
       </c>
       <c r="E2" t="n">
-        <v>56.5</v>
+        <v>74.0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0</v>
+        <v>0.5</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0</v>
+        <v>-2.0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="3">
@@ -200,22 +200,22 @@
         <v>10</v>
       </c>
       <c r="C3" t="n">
-        <v>117.0</v>
+        <v>122.0</v>
       </c>
       <c r="D3" t="n">
-        <v>56.5</v>
+        <v>65.0</v>
       </c>
       <c r="E3" t="n">
-        <v>60.5</v>
+        <v>57.0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0</v>
+        <v>13.0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0</v>
+        <v>14.0</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
     </row>
     <row r="4">
@@ -226,22 +226,22 @@
         <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>112.5</v>
+        <v>121.0</v>
       </c>
       <c r="D4" t="n">
-        <v>49.5</v>
+        <v>51.5</v>
       </c>
       <c r="E4" t="n">
-        <v>63.0</v>
+        <v>69.5</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0</v>
+        <v>-3.5</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0</v>
+        <v>-2.0</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0</v>
+        <v>-1.5</v>
       </c>
     </row>
     <row r="5">
@@ -252,22 +252,22 @@
         <v>12</v>
       </c>
       <c r="C5" t="n">
-        <v>97.0</v>
+        <v>107.0</v>
       </c>
       <c r="D5" t="n">
-        <v>24.5</v>
+        <v>66.0</v>
       </c>
       <c r="E5" t="n">
-        <v>72.5</v>
+        <v>41.0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0</v>
+        <v>6.5</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0</v>
+        <v>10.5</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0</v>
+        <v>-4.0</v>
       </c>
     </row>
     <row r="6">
@@ -278,22 +278,22 @@
         <v>13</v>
       </c>
       <c r="C6" t="n">
-        <v>95.5</v>
+        <v>89.5</v>
       </c>
       <c r="D6" t="n">
-        <v>72.5</v>
+        <v>45.0</v>
       </c>
       <c r="E6" t="n">
-        <v>23.0</v>
+        <v>44.5</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0</v>
+        <v>-2.5</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="7">
@@ -304,48 +304,48 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>95.0</v>
+        <v>88.0</v>
       </c>
       <c r="D7" t="n">
-        <v>30.0</v>
+        <v>47.5</v>
       </c>
       <c r="E7" t="n">
-        <v>65.0</v>
+        <v>40.5</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0</v>
+        <v>1.5</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
       <c r="C8" t="n">
-        <v>93.0</v>
+        <v>83.0</v>
       </c>
       <c r="D8" t="n">
         <v>49.0</v>
       </c>
       <c r="E8" t="n">
-        <v>44.0</v>
+        <v>34.0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0</v>
+        <v>0.5</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="9">
@@ -356,48 +356,48 @@
         <v>16</v>
       </c>
       <c r="C9" t="n">
-        <v>90.0</v>
+        <v>83.0</v>
       </c>
       <c r="D9" t="n">
-        <v>60.0</v>
+        <v>43.5</v>
       </c>
       <c r="E9" t="n">
-        <v>30.0</v>
+        <v>39.5</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0</v>
+        <v>-6.0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0</v>
+        <v>-2.5</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0</v>
+        <v>-3.5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
       <c r="C10" t="n">
-        <v>85.0</v>
+        <v>83.0</v>
       </c>
       <c r="D10" t="n">
-        <v>48.5</v>
+        <v>44.0</v>
       </c>
       <c r="E10" t="n">
-        <v>36.5</v>
+        <v>39.0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0</v>
+        <v>-6.0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0</v>
+        <v>-8.0</v>
       </c>
     </row>
     <row r="11">
@@ -408,74 +408,74 @@
         <v>18</v>
       </c>
       <c r="C11" t="n">
-        <v>82.5</v>
+        <v>79.0</v>
       </c>
       <c r="D11" t="n">
-        <v>46.5</v>
+        <v>20.5</v>
       </c>
       <c r="E11" t="n">
-        <v>36.0</v>
+        <v>58.5</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0</v>
+        <v>-3.0</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>11.5</v>
+        <v>11.0</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
       </c>
       <c r="C12" t="n">
-        <v>77.0</v>
+        <v>77.5</v>
       </c>
       <c r="D12" t="n">
-        <v>27.0</v>
+        <v>44.0</v>
       </c>
       <c r="E12" t="n">
-        <v>50.0</v>
+        <v>33.5</v>
       </c>
       <c r="F12" t="n">
-        <v>0.0</v>
+        <v>-13.0</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0</v>
+        <v>-9.5</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0</v>
+        <v>-3.5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>11.5</v>
+        <v>12.0</v>
       </c>
       <c r="B13" t="s">
         <v>20</v>
       </c>
       <c r="C13" t="n">
-        <v>77.0</v>
+        <v>72.0</v>
       </c>
       <c r="D13" t="n">
-        <v>43.5</v>
+        <v>32.0</v>
       </c>
       <c r="E13" t="n">
-        <v>33.5</v>
+        <v>40.0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
       <c r="G13" t="n">
-        <v>0.0</v>
+        <v>-0.5</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="14">
@@ -486,22 +486,22 @@
         <v>21</v>
       </c>
       <c r="C14" t="n">
-        <v>76.0</v>
+        <v>64.0</v>
       </c>
       <c r="D14" t="n">
-        <v>33.5</v>
+        <v>41.0</v>
       </c>
       <c r="E14" t="n">
-        <v>42.5</v>
+        <v>23.0</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0</v>
+        <v>-6.5</v>
       </c>
       <c r="G14" t="n">
-        <v>0.0</v>
+        <v>-6.0</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="15">
@@ -512,22 +512,22 @@
         <v>22</v>
       </c>
       <c r="C15" t="n">
-        <v>37.5</v>
+        <v>60.0</v>
       </c>
       <c r="D15" t="n">
-        <v>20.5</v>
+        <v>24.0</v>
       </c>
       <c r="E15" t="n">
-        <v>17.0</v>
+        <v>36.0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0</v>
+        <v>-2.0</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0</v>
+        <v>1.5</v>
       </c>
       <c r="H15" t="n">
-        <v>0.0</v>
+        <v>-3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started work on writing all excel automatically with spacing, and code clean up
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -6,13 +6,13 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Week15" r:id="rId3" sheetId="1"/>
+    <sheet name="Week22" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>rank</t>
   </si>
@@ -29,6 +29,9 @@
     <t>pitching</t>
   </si>
   <si>
+    <t>space</t>
+  </si>
+  <si>
     <t>totalChange</t>
   </si>
   <si>
@@ -47,40 +50,40 @@
     <t>EL Onće</t>
   </si>
   <si>
+    <t>Samsquanches</t>
+  </si>
+  <si>
     <t>Epic7</t>
   </si>
   <si>
-    <t>Samsquanches</t>
+    <t>GOD WILLS IT</t>
+  </si>
+  <si>
+    <t>confusion</t>
   </si>
   <si>
     <t>Splitfinger Skadoosh</t>
   </si>
   <si>
-    <t>confusion</t>
+    <t>Mac</t>
+  </si>
+  <si>
+    <t>rainmaker</t>
+  </si>
+  <si>
+    <t>Swampnuts</t>
+  </si>
+  <si>
+    <t>MillerTime</t>
   </si>
   <si>
     <t>SmokeWalkers</t>
   </si>
   <si>
-    <t>GOD WILLS IT</t>
-  </si>
-  <si>
     <t>DJ's Quality Team</t>
   </si>
   <si>
-    <t>rainmaker</t>
-  </si>
-  <si>
-    <t>Swampnuts</t>
-  </si>
-  <si>
-    <t>MillerTime</t>
-  </si>
-  <si>
     <t>Corbin Copy</t>
-  </si>
-  <si>
-    <t>Mac</t>
   </si>
 </sst>
 </file>
@@ -134,7 +137,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -165,31 +168,35 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" t="n">
-        <v>131.0</v>
+        <v>139.5</v>
       </c>
       <c r="D2" t="n">
-        <v>57.0</v>
+        <v>62.5</v>
       </c>
       <c r="E2" t="n">
-        <v>74.0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.5</v>
-      </c>
+        <v>77.0</v>
+      </c>
+      <c r="F2"/>
       <c r="G2" t="n">
-        <v>-2.0</v>
+        <v>0.11</v>
       </c>
       <c r="H2" t="n">
-        <v>2.5</v>
+        <v>0.0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="3">
@@ -197,25 +204,26 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>122.0</v>
+        <v>125.5</v>
       </c>
       <c r="D3" t="n">
-        <v>65.0</v>
+        <v>61.5</v>
       </c>
       <c r="E3" t="n">
-        <v>57.0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>13.0</v>
-      </c>
+        <v>64.0</v>
+      </c>
+      <c r="F3"/>
       <c r="G3" t="n">
-        <v>14.0</v>
+        <v>0.11</v>
       </c>
       <c r="H3" t="n">
-        <v>-1.0</v>
+        <v>0.0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
@@ -223,25 +231,26 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="n">
-        <v>121.0</v>
+        <v>103.5</v>
       </c>
       <c r="D4" t="n">
-        <v>51.5</v>
+        <v>57.0</v>
       </c>
       <c r="E4" t="n">
-        <v>69.5</v>
-      </c>
-      <c r="F4" t="n">
-        <v>-3.5</v>
-      </c>
+        <v>46.5</v>
+      </c>
+      <c r="F4"/>
       <c r="G4" t="n">
-        <v>-2.0</v>
+        <v>0.11</v>
       </c>
       <c r="H4" t="n">
-        <v>-1.5</v>
+        <v>0.0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
@@ -249,25 +258,26 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="n">
-        <v>107.0</v>
+        <v>96.5</v>
       </c>
       <c r="D5" t="n">
-        <v>66.0</v>
+        <v>38.5</v>
       </c>
       <c r="E5" t="n">
-        <v>41.0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>6.5</v>
-      </c>
+        <v>58.0</v>
+      </c>
+      <c r="F5"/>
       <c r="G5" t="n">
-        <v>10.5</v>
+        <v>0.11</v>
       </c>
       <c r="H5" t="n">
-        <v>-4.0</v>
+        <v>0.0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="6">
@@ -275,25 +285,26 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>89.5</v>
+        <v>91.5</v>
       </c>
       <c r="D6" t="n">
-        <v>45.0</v>
+        <v>48.5</v>
       </c>
       <c r="E6" t="n">
-        <v>44.5</v>
-      </c>
-      <c r="F6" t="n">
-        <v>7.0</v>
-      </c>
+        <v>43.0</v>
+      </c>
+      <c r="F6"/>
       <c r="G6" t="n">
-        <v>-2.5</v>
+        <v>0.11</v>
       </c>
       <c r="H6" t="n">
-        <v>9.5</v>
+        <v>0.0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="7">
@@ -301,51 +312,53 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" t="n">
-        <v>88.0</v>
+        <v>89.5</v>
       </c>
       <c r="D7" t="n">
-        <v>47.5</v>
+        <v>57.5</v>
       </c>
       <c r="E7" t="n">
-        <v>40.5</v>
-      </c>
-      <c r="F7" t="n">
-        <v>1.5</v>
-      </c>
+        <v>32.0</v>
+      </c>
+      <c r="F7"/>
       <c r="G7" t="n">
-        <v>1.0</v>
+        <v>0.11</v>
       </c>
       <c r="H7" t="n">
-        <v>0.5</v>
+        <v>0.0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>83.0</v>
+        <v>86.0</v>
       </c>
       <c r="D8" t="n">
-        <v>49.0</v>
+        <v>36.5</v>
       </c>
       <c r="E8" t="n">
-        <v>34.0</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.5</v>
-      </c>
+        <v>49.5</v>
+      </c>
+      <c r="F8"/>
       <c r="G8" t="n">
-        <v>-1.0</v>
+        <v>0.11</v>
       </c>
       <c r="H8" t="n">
-        <v>1.5</v>
+        <v>0.0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="9">
@@ -353,51 +366,53 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" t="n">
-        <v>83.0</v>
+        <v>85.5</v>
       </c>
       <c r="D9" t="n">
-        <v>43.5</v>
+        <v>44.5</v>
       </c>
       <c r="E9" t="n">
-        <v>39.5</v>
-      </c>
-      <c r="F9" t="n">
-        <v>-6.0</v>
-      </c>
+        <v>41.0</v>
+      </c>
+      <c r="F9"/>
       <c r="G9" t="n">
-        <v>-2.5</v>
+        <v>0.11</v>
       </c>
       <c r="H9" t="n">
-        <v>-3.5</v>
+        <v>0.0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" t="n">
         <v>83.0</v>
       </c>
       <c r="D10" t="n">
-        <v>44.0</v>
+        <v>24.0</v>
       </c>
       <c r="E10" t="n">
-        <v>39.0</v>
-      </c>
-      <c r="F10" t="n">
-        <v>-6.0</v>
-      </c>
+        <v>59.0</v>
+      </c>
+      <c r="F10"/>
       <c r="G10" t="n">
-        <v>2.0</v>
+        <v>0.11</v>
       </c>
       <c r="H10" t="n">
-        <v>-8.0</v>
+        <v>0.0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="11">
@@ -405,25 +420,26 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C11" t="n">
-        <v>79.0</v>
+        <v>81.0</v>
       </c>
       <c r="D11" t="n">
-        <v>20.5</v>
+        <v>37.5</v>
       </c>
       <c r="E11" t="n">
-        <v>58.5</v>
-      </c>
-      <c r="F11" t="n">
-        <v>-1.0</v>
-      </c>
+        <v>43.5</v>
+      </c>
+      <c r="F11"/>
       <c r="G11" t="n">
-        <v>-3.0</v>
+        <v>0.11</v>
       </c>
       <c r="H11" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="12">
@@ -431,25 +447,26 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C12" t="n">
-        <v>77.5</v>
+        <v>74.0</v>
       </c>
       <c r="D12" t="n">
-        <v>44.0</v>
+        <v>36.5</v>
       </c>
       <c r="E12" t="n">
-        <v>33.5</v>
-      </c>
-      <c r="F12" t="n">
-        <v>-13.0</v>
-      </c>
+        <v>37.5</v>
+      </c>
+      <c r="F12"/>
       <c r="G12" t="n">
-        <v>-9.5</v>
+        <v>0.11</v>
       </c>
       <c r="H12" t="n">
-        <v>-3.5</v>
+        <v>0.0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="13">
@@ -457,25 +474,26 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C13" t="n">
-        <v>72.0</v>
+        <v>73.5</v>
       </c>
       <c r="D13" t="n">
-        <v>32.0</v>
+        <v>38.5</v>
       </c>
       <c r="E13" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="F13" t="n">
-        <v>9.0</v>
-      </c>
+        <v>35.0</v>
+      </c>
+      <c r="F13"/>
       <c r="G13" t="n">
-        <v>-0.5</v>
+        <v>0.11</v>
       </c>
       <c r="H13" t="n">
-        <v>9.5</v>
+        <v>0.0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="14">
@@ -483,25 +501,26 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14" t="n">
-        <v>64.0</v>
+        <v>68.0</v>
       </c>
       <c r="D14" t="n">
-        <v>41.0</v>
+        <v>41.5</v>
       </c>
       <c r="E14" t="n">
-        <v>23.0</v>
-      </c>
-      <c r="F14" t="n">
-        <v>-6.5</v>
-      </c>
+        <v>26.5</v>
+      </c>
+      <c r="F14"/>
       <c r="G14" t="n">
-        <v>-6.0</v>
+        <v>0.11</v>
       </c>
       <c r="H14" t="n">
-        <v>-0.5</v>
+        <v>0.0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="15">
@@ -509,25 +528,26 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C15" t="n">
-        <v>60.0</v>
+        <v>63.0</v>
       </c>
       <c r="D15" t="n">
-        <v>24.0</v>
+        <v>45.5</v>
       </c>
       <c r="E15" t="n">
-        <v>36.0</v>
-      </c>
-      <c r="F15" t="n">
-        <v>-2.0</v>
-      </c>
+        <v>17.5</v>
+      </c>
+      <c r="F15"/>
       <c r="G15" t="n">
-        <v>1.5</v>
+        <v>0.11</v>
       </c>
       <c r="H15" t="n">
-        <v>-3.5</v>
+        <v>0.0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
succeeded in auto printing hitting and pitching ranks
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -6,13 +6,13 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Week22" r:id="rId3" sheetId="1"/>
+    <sheet name="Sheet" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="25">
   <si>
     <t>rank</t>
   </si>
@@ -32,13 +32,13 @@
     <t>space</t>
   </si>
   <si>
-    <t>totalChange</t>
-  </si>
-  <si>
-    <t>hittingChange</t>
-  </si>
-  <si>
-    <t>pitchingChange</t>
+    <t>total_change</t>
+  </si>
+  <si>
+    <t>hitting_change</t>
+  </si>
+  <si>
+    <t>pitching_change</t>
   </si>
   <si>
     <t/>
@@ -62,15 +62,15 @@
     <t>confusion</t>
   </si>
   <si>
+    <t>rainmaker</t>
+  </si>
+  <si>
+    <t>Mac</t>
+  </si>
+  <si>
     <t>Splitfinger Skadoosh</t>
   </si>
   <si>
-    <t>Mac</t>
-  </si>
-  <si>
-    <t>rainmaker</t>
-  </si>
-  <si>
     <t>Swampnuts</t>
   </si>
   <si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Corbin Copy</t>
+  </si>
+  <si>
+    <t>name_</t>
   </si>
 </sst>
 </file>
@@ -137,7 +140,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -288,13 +291,13 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>91.5</v>
+        <v>90.5</v>
       </c>
       <c r="D6" t="n">
         <v>48.5</v>
       </c>
       <c r="E6" t="n">
-        <v>43.0</v>
+        <v>42.0</v>
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
@@ -345,10 +348,10 @@
         <v>86.0</v>
       </c>
       <c r="D8" t="n">
-        <v>36.5</v>
+        <v>24.0</v>
       </c>
       <c r="E8" t="n">
-        <v>49.5</v>
+        <v>62.0</v>
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
@@ -396,13 +399,13 @@
         <v>18</v>
       </c>
       <c r="C10" t="n">
-        <v>83.0</v>
+        <v>85.0</v>
       </c>
       <c r="D10" t="n">
-        <v>24.0</v>
+        <v>36.5</v>
       </c>
       <c r="E10" t="n">
-        <v>59.0</v>
+        <v>48.5</v>
       </c>
       <c r="F10"/>
       <c r="G10" t="n">
@@ -504,13 +507,13 @@
         <v>22</v>
       </c>
       <c r="C14" t="n">
-        <v>68.0</v>
+        <v>67.0</v>
       </c>
       <c r="D14" t="n">
         <v>41.5</v>
       </c>
       <c r="E14" t="n">
-        <v>26.5</v>
+        <v>25.5</v>
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
@@ -548,6 +551,281 @@
       </c>
       <c r="I15" t="n">
         <v>0.0</v>
+      </c>
+    </row>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="D20"/>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" t="n">
+        <v>77.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="n">
+        <v>61.5</v>
+      </c>
+      <c r="D21"/>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" t="n">
+        <v>64.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" t="n">
+        <v>57.0</v>
+      </c>
+      <c r="D22"/>
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" t="n">
+        <v>46.5</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="n">
+        <v>38.5</v>
+      </c>
+      <c r="D23"/>
+      <c r="E23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" t="n">
+        <v>58.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" t="n">
+        <v>48.5</v>
+      </c>
+      <c r="D24"/>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" t="n">
+        <v>42.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" t="n">
+        <v>57.5</v>
+      </c>
+      <c r="D25"/>
+      <c r="E25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="D26"/>
+      <c r="E26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" t="n">
+        <v>62.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" t="n">
+        <v>44.5</v>
+      </c>
+      <c r="D27"/>
+      <c r="E27" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" t="n">
+        <v>41.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" t="n">
+        <v>36.5</v>
+      </c>
+      <c r="D28"/>
+      <c r="E28" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" t="n">
+        <v>48.5</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="D29"/>
+      <c r="E29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" t="n">
+        <v>43.5</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" t="n">
+        <v>36.5</v>
+      </c>
+      <c r="D30"/>
+      <c r="E30" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" t="n">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" t="n">
+        <v>38.5</v>
+      </c>
+      <c r="D31"/>
+      <c r="E31" t="s">
+        <v>21</v>
+      </c>
+      <c r="F31" t="n">
+        <v>35.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" t="n">
+        <v>41.5</v>
+      </c>
+      <c r="D32"/>
+      <c r="E32" t="s">
+        <v>22</v>
+      </c>
+      <c r="F32" t="n">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="D33"/>
+      <c r="E33" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" t="n">
+        <v>17.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated to be able to print two tables while also reading from same sheet
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="27">
   <si>
     <t>rank</t>
   </si>
@@ -50,6 +50,9 @@
     <t>EL Onće</t>
   </si>
   <si>
+    <t>rainmaker</t>
+  </si>
+  <si>
     <t>Samsquanches</t>
   </si>
   <si>
@@ -62,9 +65,6 @@
     <t>confusion</t>
   </si>
   <si>
-    <t>rainmaker</t>
-  </si>
-  <si>
     <t>Mac</t>
   </si>
   <si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>Corbin Copy</t>
+  </si>
+  <si>
+    <t>hitting_rank</t>
+  </si>
+  <si>
+    <t>pitching_rank</t>
   </si>
   <si>
     <t>name_</t>
@@ -183,20 +189,20 @@
         <v>10</v>
       </c>
       <c r="C2" t="n">
-        <v>139.5</v>
+        <v>138.5</v>
       </c>
       <c r="D2" t="n">
-        <v>62.5</v>
+        <v>61.5</v>
       </c>
       <c r="E2" t="n">
         <v>77.0</v>
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>0.11</v>
+        <v>-1.0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="I2" t="n">
         <v>0.0</v>
@@ -210,20 +216,20 @@
         <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>125.5</v>
+        <v>123.5</v>
       </c>
       <c r="D3" t="n">
-        <v>61.5</v>
+        <v>59.5</v>
       </c>
       <c r="E3" t="n">
         <v>64.0</v>
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.11</v>
+        <v>-2.0</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0</v>
+        <v>-2.0</v>
       </c>
       <c r="I3" t="n">
         <v>0.0</v>
@@ -237,20 +243,20 @@
         <v>12</v>
       </c>
       <c r="C4" t="n">
-        <v>103.5</v>
+        <v>103.0</v>
       </c>
       <c r="D4" t="n">
-        <v>57.0</v>
+        <v>41.0</v>
       </c>
       <c r="E4" t="n">
-        <v>46.5</v>
+        <v>62.0</v>
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.11</v>
+        <v>17.0</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0</v>
+        <v>17.0</v>
       </c>
       <c r="I4" t="n">
         <v>0.0</v>
@@ -264,20 +270,20 @@
         <v>13</v>
       </c>
       <c r="C5" t="n">
-        <v>96.5</v>
+        <v>102.5</v>
       </c>
       <c r="D5" t="n">
-        <v>38.5</v>
+        <v>56.0</v>
       </c>
       <c r="E5" t="n">
-        <v>58.0</v>
+        <v>46.5</v>
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.11</v>
+        <v>-1.0</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="I5" t="n">
         <v>0.0</v>
@@ -291,20 +297,20 @@
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>90.5</v>
+        <v>95.5</v>
       </c>
       <c r="D6" t="n">
-        <v>48.5</v>
+        <v>37.5</v>
       </c>
       <c r="E6" t="n">
-        <v>42.0</v>
+        <v>58.0</v>
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.11</v>
+        <v>-1.0</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="I6" t="n">
         <v>0.0</v>
@@ -312,26 +318,26 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6.0</v>
+        <v>6.5</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
       <c r="C7" t="n">
-        <v>89.5</v>
+        <v>88.5</v>
       </c>
       <c r="D7" t="n">
-        <v>57.5</v>
+        <v>46.5</v>
       </c>
       <c r="E7" t="n">
-        <v>32.0</v>
+        <v>42.0</v>
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.11</v>
+        <v>-2.0</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0</v>
+        <v>-2.0</v>
       </c>
       <c r="I7" t="n">
         <v>0.0</v>
@@ -339,26 +345,26 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7.0</v>
+        <v>6.5</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>86.0</v>
+        <v>88.5</v>
       </c>
       <c r="D8" t="n">
-        <v>24.0</v>
+        <v>56.5</v>
       </c>
       <c r="E8" t="n">
-        <v>62.0</v>
+        <v>32.0</v>
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.11</v>
+        <v>-1.0</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="I8" t="n">
         <v>0.0</v>
@@ -372,20 +378,20 @@
         <v>17</v>
       </c>
       <c r="C9" t="n">
-        <v>85.5</v>
+        <v>84.5</v>
       </c>
       <c r="D9" t="n">
-        <v>44.5</v>
+        <v>43.5</v>
       </c>
       <c r="E9" t="n">
         <v>41.0</v>
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.11</v>
+        <v>-1.0</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="I9" t="n">
         <v>0.0</v>
@@ -399,20 +405,20 @@
         <v>18</v>
       </c>
       <c r="C10" t="n">
-        <v>85.0</v>
+        <v>83.0</v>
       </c>
       <c r="D10" t="n">
-        <v>36.5</v>
+        <v>34.5</v>
       </c>
       <c r="E10" t="n">
         <v>48.5</v>
       </c>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>0.11</v>
+        <v>-2.0</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0</v>
+        <v>-2.0</v>
       </c>
       <c r="I10" t="n">
         <v>0.0</v>
@@ -426,20 +432,20 @@
         <v>19</v>
       </c>
       <c r="C11" t="n">
-        <v>81.0</v>
+        <v>79.0</v>
       </c>
       <c r="D11" t="n">
-        <v>37.5</v>
+        <v>35.5</v>
       </c>
       <c r="E11" t="n">
         <v>43.5</v>
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>0.11</v>
+        <v>-2.0</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0</v>
+        <v>-2.0</v>
       </c>
       <c r="I11" t="n">
         <v>0.0</v>
@@ -463,7 +469,7 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>0.11</v>
+        <v>0.0</v>
       </c>
       <c r="H12" t="n">
         <v>0.0</v>
@@ -480,20 +486,20 @@
         <v>21</v>
       </c>
       <c r="C13" t="n">
-        <v>73.5</v>
+        <v>72.5</v>
       </c>
       <c r="D13" t="n">
-        <v>38.5</v>
+        <v>37.5</v>
       </c>
       <c r="E13" t="n">
         <v>35.0</v>
       </c>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>0.11</v>
+        <v>-1.0</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="I13" t="n">
         <v>0.0</v>
@@ -507,20 +513,20 @@
         <v>22</v>
       </c>
       <c r="C14" t="n">
-        <v>67.0</v>
+        <v>66.0</v>
       </c>
       <c r="D14" t="n">
-        <v>41.5</v>
+        <v>40.5</v>
       </c>
       <c r="E14" t="n">
         <v>25.5</v>
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>0.11</v>
+        <v>-1.0</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="I14" t="n">
         <v>0.0</v>
@@ -534,20 +540,20 @@
         <v>23</v>
       </c>
       <c r="C15" t="n">
-        <v>63.0</v>
+        <v>61.0</v>
       </c>
       <c r="D15" t="n">
-        <v>45.5</v>
+        <v>43.5</v>
       </c>
       <c r="E15" t="n">
         <v>17.5</v>
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>0.11</v>
+        <v>-2.0</v>
       </c>
       <c r="H15" t="n">
-        <v>0.0</v>
+        <v>-2.0</v>
       </c>
       <c r="I15" t="n">
         <v>0.0</v>
@@ -558,7 +564,7 @@
     <row r="18"/>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>1</v>
@@ -570,9 +576,12 @@
         <v>5</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -584,13 +593,16 @@
         <v>10</v>
       </c>
       <c r="C20" t="n">
-        <v>62.5</v>
+        <v>61.5</v>
       </c>
       <c r="D20"/>
-      <c r="E20" t="s">
+      <c r="E20" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F20" t="s">
         <v>10</v>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>77.0</v>
       </c>
     </row>
@@ -602,13 +614,16 @@
         <v>11</v>
       </c>
       <c r="C21" t="n">
-        <v>61.5</v>
+        <v>59.5</v>
       </c>
       <c r="D21"/>
-      <c r="E21" t="s">
+      <c r="E21" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F21" t="s">
         <v>11</v>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>64.0</v>
       </c>
     </row>
@@ -617,17 +632,20 @@
         <v>3.0</v>
       </c>
       <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="n">
+        <v>56.5</v>
+      </c>
+      <c r="D22"/>
+      <c r="E22" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F22" t="s">
         <v>12</v>
       </c>
-      <c r="C22" t="n">
-        <v>57.0</v>
-      </c>
-      <c r="D22"/>
-      <c r="E22" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" t="n">
-        <v>46.5</v>
+      <c r="G22" t="n">
+        <v>62.0</v>
       </c>
     </row>
     <row r="23">
@@ -638,13 +656,16 @@
         <v>13</v>
       </c>
       <c r="C23" t="n">
-        <v>38.5</v>
+        <v>56.0</v>
       </c>
       <c r="D23"/>
-      <c r="E23" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" t="n">
+      <c r="E23" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" t="n">
         <v>58.0</v>
       </c>
     </row>
@@ -653,17 +674,20 @@
         <v>5.0</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C24" t="n">
+        <v>46.5</v>
+      </c>
+      <c r="D24"/>
+      <c r="E24" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" t="n">
         <v>48.5</v>
-      </c>
-      <c r="D24"/>
-      <c r="E24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" t="n">
-        <v>42.0</v>
       </c>
     </row>
     <row r="25">
@@ -671,17 +695,20 @@
         <v>6.0</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C25" t="n">
-        <v>57.5</v>
+        <v>43.5</v>
       </c>
       <c r="D25"/>
-      <c r="E25" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" t="n">
-        <v>32.0</v>
+      <c r="E25" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" t="n">
+        <v>46.5</v>
       </c>
     </row>
     <row r="26">
@@ -689,17 +716,20 @@
         <v>7.0</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C26" t="n">
-        <v>24.0</v>
+        <v>43.5</v>
       </c>
       <c r="D26"/>
-      <c r="E26" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" t="n">
-        <v>62.0</v>
+      <c r="E26" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" t="n">
+        <v>43.5</v>
       </c>
     </row>
     <row r="27">
@@ -707,17 +737,20 @@
         <v>8.0</v>
       </c>
       <c r="B27" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C27" t="n">
-        <v>44.5</v>
+        <v>41.0</v>
       </c>
       <c r="D27"/>
-      <c r="E27" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27" t="n">
-        <v>41.0</v>
+      <c r="E27" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" t="n">
+        <v>42.0</v>
       </c>
     </row>
     <row r="28">
@@ -725,17 +758,20 @@
         <v>9.0</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C28" t="n">
-        <v>36.5</v>
+        <v>40.5</v>
       </c>
       <c r="D28"/>
-      <c r="E28" t="s">
-        <v>18</v>
-      </c>
-      <c r="F28" t="n">
-        <v>48.5</v>
+      <c r="E28" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" t="n">
+        <v>41.0</v>
       </c>
     </row>
     <row r="29">
@@ -743,17 +779,20 @@
         <v>10.0</v>
       </c>
       <c r="B29" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C29" t="n">
         <v>37.5</v>
       </c>
       <c r="D29"/>
-      <c r="E29" t="s">
-        <v>19</v>
-      </c>
-      <c r="F29" t="n">
-        <v>43.5</v>
+      <c r="E29" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" t="n">
+        <v>37.5</v>
       </c>
     </row>
     <row r="30">
@@ -761,17 +800,20 @@
         <v>11.0</v>
       </c>
       <c r="B30" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C30" t="n">
-        <v>36.5</v>
+        <v>37.5</v>
       </c>
       <c r="D30"/>
-      <c r="E30" t="s">
-        <v>20</v>
-      </c>
-      <c r="F30" t="n">
-        <v>37.5</v>
+      <c r="E30" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>21</v>
+      </c>
+      <c r="G30" t="n">
+        <v>35.0</v>
       </c>
     </row>
     <row r="31">
@@ -779,17 +821,20 @@
         <v>12.0</v>
       </c>
       <c r="B31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C31" t="n">
-        <v>38.5</v>
+        <v>36.5</v>
       </c>
       <c r="D31"/>
-      <c r="E31" t="s">
-        <v>21</v>
-      </c>
-      <c r="F31" t="n">
-        <v>35.0</v>
+      <c r="E31" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" t="n">
+        <v>32.0</v>
       </c>
     </row>
     <row r="32">
@@ -797,16 +842,19 @@
         <v>13.0</v>
       </c>
       <c r="B32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" t="n">
+        <v>35.5</v>
+      </c>
+      <c r="D32"/>
+      <c r="E32" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="F32" t="s">
         <v>22</v>
       </c>
-      <c r="C32" t="n">
-        <v>41.5</v>
-      </c>
-      <c r="D32"/>
-      <c r="E32" t="s">
-        <v>22</v>
-      </c>
-      <c r="F32" t="n">
+      <c r="G32" t="n">
         <v>25.5</v>
       </c>
     </row>
@@ -815,16 +863,19 @@
         <v>14.0</v>
       </c>
       <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" t="n">
+        <v>34.5</v>
+      </c>
+      <c r="D33"/>
+      <c r="E33" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="F33" t="s">
         <v>23</v>
       </c>
-      <c r="C33" t="n">
-        <v>45.5</v>
-      </c>
-      <c r="D33"/>
-      <c r="E33" t="s">
-        <v>23</v>
-      </c>
-      <c r="F33" t="n">
+      <c r="G33" t="n">
         <v>17.5</v>
       </c>
     </row>

</xml_diff>